<commit_message>
refine verb selection and adjust speech rate
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C336A955-C04F-4645-95F9-62558BFEF9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239C9E7A-1FD0-46BE-AF7E-CB8D8F9B24BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="416">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -54,12 +54,6 @@
     <t>行く</t>
   </si>
   <si>
-    <t>行って</t>
-  </si>
-  <si>
-    <t>行った</t>
-  </si>
-  <si>
     <t>行かない</t>
   </si>
   <si>
@@ -1329,6 +1323,70 @@
   </si>
   <si>
     <t>渡そう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>いって</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>いった</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返す</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返して</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返した</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返さない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返します</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返そう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼く</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼いて</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼いた</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼かない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼きます</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼こう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>座ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>乗ろう</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1396,7 +1454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1406,6 +1464,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1720,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1750,10 +1811,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
@@ -1770,1531 +1831,1574 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>372</v>
+      <c r="F13" s="3" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>87</v>
       </c>
-      <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>85</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
         <v>77</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>79</v>
       </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
         <v>110</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>111</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>112</v>
       </c>
-      <c r="D23" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" t="s">
-        <v>114</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>116</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>117</v>
       </c>
-      <c r="D24" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" t="s">
-        <v>119</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
         <v>120</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>121</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>122</v>
       </c>
-      <c r="D25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" t="s">
-        <v>124</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
         <v>125</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>126</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>127</v>
       </c>
-      <c r="D26" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" t="s">
-        <v>129</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="s">
         <v>130</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>132</v>
       </c>
-      <c r="D27" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" t="s">
-        <v>134</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" t="s">
         <v>135</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>136</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>137</v>
       </c>
-      <c r="D28" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" t="s">
-        <v>139</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s">
         <v>140</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>141</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>142</v>
       </c>
-      <c r="D29" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" t="s">
-        <v>144</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" t="s">
         <v>145</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>146</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>147</v>
       </c>
-      <c r="D30" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" t="s">
-        <v>149</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" t="s">
         <v>150</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>151</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>152</v>
       </c>
-      <c r="D31" t="s">
-        <v>153</v>
-      </c>
-      <c r="E31" t="s">
-        <v>154</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" t="s">
         <v>155</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>156</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>157</v>
       </c>
-      <c r="D32" t="s">
-        <v>158</v>
-      </c>
-      <c r="E32" t="s">
-        <v>159</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
         <v>160</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>161</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>162</v>
       </c>
-      <c r="D33" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" t="s">
-        <v>164</v>
-      </c>
       <c r="F33" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" t="s">
         <v>165</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>166</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>167</v>
       </c>
-      <c r="D34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" t="s">
-        <v>169</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" t="s">
         <v>170</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>171</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>172</v>
       </c>
-      <c r="D35" t="s">
-        <v>173</v>
-      </c>
-      <c r="E35" t="s">
-        <v>174</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" t="s">
         <v>175</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>176</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>177</v>
       </c>
-      <c r="D36" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" t="s">
-        <v>179</v>
-      </c>
       <c r="F36" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" t="s">
         <v>180</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>181</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>182</v>
       </c>
-      <c r="D37" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" t="s">
-        <v>184</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
         <v>185</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>186</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>187</v>
       </c>
-      <c r="D38" t="s">
-        <v>188</v>
-      </c>
-      <c r="E38" t="s">
-        <v>189</v>
-      </c>
       <c r="F38" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" t="s">
         <v>190</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>191</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>192</v>
       </c>
-      <c r="D39" t="s">
-        <v>193</v>
-      </c>
-      <c r="E39" t="s">
-        <v>194</v>
-      </c>
       <c r="F39" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" t="s">
         <v>195</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>196</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>197</v>
       </c>
-      <c r="D40" t="s">
-        <v>198</v>
-      </c>
-      <c r="E40" t="s">
-        <v>199</v>
-      </c>
       <c r="F40" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41" t="s">
+        <v>199</v>
+      </c>
+      <c r="C41" t="s">
         <v>200</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>201</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>202</v>
       </c>
-      <c r="D41" t="s">
-        <v>203</v>
-      </c>
-      <c r="E41" t="s">
-        <v>204</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" t="s">
         <v>205</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>206</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>207</v>
       </c>
-      <c r="D42" t="s">
-        <v>208</v>
-      </c>
-      <c r="E42" t="s">
-        <v>209</v>
-      </c>
       <c r="F42" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" t="s">
+        <v>209</v>
+      </c>
+      <c r="C43" t="s">
         <v>210</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>211</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
         <v>212</v>
       </c>
-      <c r="D43" t="s">
-        <v>213</v>
-      </c>
-      <c r="E43" t="s">
-        <v>214</v>
-      </c>
       <c r="F43" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
         <v>60</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>61</v>
       </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
         <v>62</v>
       </c>
-      <c r="D44" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" t="s">
-        <v>64</v>
-      </c>
       <c r="F44" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" t="s">
         <v>215</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>216</v>
       </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
         <v>217</v>
       </c>
-      <c r="D45" t="s">
-        <v>218</v>
-      </c>
-      <c r="E45" t="s">
-        <v>219</v>
-      </c>
       <c r="F45" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" t="s">
         <v>220</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>221</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
         <v>222</v>
       </c>
-      <c r="D46" t="s">
-        <v>223</v>
-      </c>
-      <c r="E46" t="s">
-        <v>224</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>223</v>
+      </c>
+      <c r="B47" t="s">
+        <v>224</v>
+      </c>
+      <c r="C47" t="s">
         <v>225</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>226</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>227</v>
       </c>
-      <c r="D47" t="s">
-        <v>228</v>
-      </c>
-      <c r="E47" t="s">
-        <v>229</v>
-      </c>
       <c r="F47" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" t="s">
+        <v>229</v>
+      </c>
+      <c r="C48" t="s">
         <v>230</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>231</v>
       </c>
-      <c r="C48" t="s">
+      <c r="E48" t="s">
         <v>232</v>
       </c>
-      <c r="D48" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" t="s">
-        <v>234</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" t="s">
         <v>235</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>236</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>237</v>
       </c>
-      <c r="D49" t="s">
-        <v>238</v>
-      </c>
-      <c r="E49" t="s">
-        <v>239</v>
-      </c>
       <c r="F49" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" t="s">
+        <v>239</v>
+      </c>
+      <c r="C50" t="s">
         <v>240</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>241</v>
       </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
         <v>242</v>
       </c>
-      <c r="D50" t="s">
-        <v>243</v>
-      </c>
-      <c r="E50" t="s">
-        <v>244</v>
-      </c>
       <c r="F50" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" t="s">
+        <v>244</v>
+      </c>
+      <c r="C51" t="s">
         <v>245</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>246</v>
       </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>247</v>
       </c>
-      <c r="D51" t="s">
-        <v>248</v>
-      </c>
-      <c r="E51" t="s">
-        <v>249</v>
-      </c>
       <c r="F51" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>248</v>
+      </c>
+      <c r="B52" t="s">
+        <v>249</v>
+      </c>
+      <c r="C52" t="s">
         <v>250</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>251</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>252</v>
       </c>
-      <c r="D52" t="s">
-        <v>253</v>
-      </c>
-      <c r="E52" t="s">
-        <v>254</v>
-      </c>
       <c r="F52" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>253</v>
+      </c>
+      <c r="B53" t="s">
+        <v>254</v>
+      </c>
+      <c r="C53" t="s">
         <v>255</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>256</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>257</v>
       </c>
-      <c r="D53" t="s">
-        <v>258</v>
-      </c>
-      <c r="E53" t="s">
-        <v>259</v>
-      </c>
       <c r="F53" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>258</v>
+      </c>
+      <c r="B54" t="s">
+        <v>259</v>
+      </c>
+      <c r="C54" t="s">
         <v>260</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>261</v>
       </c>
-      <c r="C54" t="s">
+      <c r="E54" t="s">
         <v>262</v>
       </c>
-      <c r="D54" t="s">
-        <v>263</v>
-      </c>
-      <c r="E54" t="s">
-        <v>264</v>
-      </c>
       <c r="F54" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55" t="s">
+        <v>264</v>
+      </c>
+      <c r="C55" t="s">
         <v>265</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>266</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
         <v>267</v>
       </c>
-      <c r="D55" t="s">
-        <v>268</v>
-      </c>
-      <c r="E55" t="s">
-        <v>269</v>
-      </c>
       <c r="F55" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>268</v>
+      </c>
+      <c r="B56" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" t="s">
         <v>270</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>271</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
         <v>272</v>
       </c>
-      <c r="D56" t="s">
-        <v>273</v>
-      </c>
-      <c r="E56" t="s">
-        <v>274</v>
-      </c>
       <c r="F56" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>273</v>
+      </c>
+      <c r="B57" t="s">
+        <v>274</v>
+      </c>
+      <c r="C57" t="s">
         <v>275</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>276</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>277</v>
       </c>
-      <c r="D57" t="s">
-        <v>278</v>
-      </c>
-      <c r="E57" t="s">
-        <v>279</v>
-      </c>
       <c r="F57" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>278</v>
+      </c>
+      <c r="B58" t="s">
+        <v>279</v>
+      </c>
+      <c r="C58" t="s">
         <v>280</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>281</v>
       </c>
-      <c r="C58" t="s">
+      <c r="E58" t="s">
         <v>282</v>
       </c>
-      <c r="D58" t="s">
-        <v>283</v>
-      </c>
-      <c r="E58" t="s">
-        <v>284</v>
-      </c>
       <c r="F58" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>283</v>
+      </c>
+      <c r="B59" t="s">
+        <v>284</v>
+      </c>
+      <c r="C59" t="s">
         <v>285</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>286</v>
       </c>
-      <c r="C59" t="s">
+      <c r="E59" t="s">
         <v>287</v>
       </c>
-      <c r="D59" t="s">
-        <v>288</v>
-      </c>
-      <c r="E59" t="s">
-        <v>289</v>
-      </c>
       <c r="F59" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>294</v>
-      </c>
       <c r="F60" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>299</v>
-      </c>
       <c r="F61" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="F62" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>309</v>
-      </c>
       <c r="F63" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>314</v>
-      </c>
       <c r="F64" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="F65" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="F66" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="F67" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>334</v>
-      </c>
       <c r="F68" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>339</v>
-      </c>
       <c r="F69" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>344</v>
-      </c>
       <c r="F70" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>354</v>
-      </c>
       <c r="F71" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>359</v>
-      </c>
       <c r="F72" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="F73" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>377</v>
-      </c>
       <c r="F74" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="F75" s="4" t="s">
         <v>381</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="F76" s="4" t="s">
         <v>387</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="F77" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>401</v>
-      </c>
+    </row>
+    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A79" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A81" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
enhance verb selection and tracking with cookie support; add reset functionality
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E736CE07-1530-467E-87D3-82402D3D0E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDE30C6-DA62-4CF5-ADD4-3494E03D5459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="461">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -1418,10 +1418,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>とわわない</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>とおります</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1435,6 +1431,142 @@
   </si>
   <si>
     <t>かよおう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送る</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下る</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>通わない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送らない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送ります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がって</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がった</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がらない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下らない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下ります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がって</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がった</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がらない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>始まろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>困ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>謝ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集まる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集まって</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集まった</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集まらない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集まります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集まろう</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1829,10 +1961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3281,8 +3413,8 @@
       <c r="E72" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>370</v>
+      <c r="F72" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
@@ -3301,8 +3433,8 @@
       <c r="E73" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="F73" s="4" t="s">
-        <v>370</v>
+      <c r="F73" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
@@ -3321,8 +3453,8 @@
       <c r="E74" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="F74" s="4" t="s">
-        <v>370</v>
+      <c r="F74" s="3" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
@@ -3459,10 +3591,10 @@
         <v>422</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
@@ -3476,13 +3608,113 @@
         <v>421</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F82" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A83" s="3" t="s">
         <v>427</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A84" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A85" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A86" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A87" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor verb selection logic and update frontend interaction; remove cookie dependency and enhance session management
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDE30C6-DA62-4CF5-ADD4-3494E03D5459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA42EC8-DE62-4C1B-94FE-887BCC45334D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="472">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -1567,6 +1567,50 @@
   </si>
   <si>
     <t>集まろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>会う</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>会って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>あった</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>会わない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>会います</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>会おう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>言う</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>言って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>言った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>言わない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>言います</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1961,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3717,6 +3761,46 @@
         <v>460</v>
       </c>
     </row>
+    <row r="88" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A88" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A89" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Volitional Form support
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mptang\Desktop\local testing\online-web-app-deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA42EC8-DE62-4C1B-94FE-887BCC45334D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287B3742-7A94-4633-A85D-C95D70C9F1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="32565" yWindow="4020" windowWidth="21600" windowHeight="11295" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="474">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -1612,17 +1612,23 @@
   <si>
     <t>言います</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>払おう</t>
+  </si>
+  <si>
+    <t>渡ろう</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1631,14 +1637,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1693,7 +1699,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1709,9 +1715,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1749,7 +1755,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1855,7 +1861,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1997,7 +2003,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2007,11 +2013,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -2021,7 +2027,7 @@
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2047,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2061,7 +2067,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2101,7 +2107,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2161,7 +2167,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="18.75">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -2201,7 +2207,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -2221,7 +2227,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -2241,7 +2247,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -2301,7 +2307,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -2321,7 +2327,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2481,7 +2487,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -2521,7 +2527,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -2601,7 +2607,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -2641,7 +2647,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -2681,7 +2687,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -2701,7 +2707,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -2721,7 +2727,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>173</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>178</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>188</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>193</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -2841,7 +2847,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>203</v>
       </c>
@@ -2861,7 +2867,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>208</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>213</v>
       </c>
@@ -2921,7 +2927,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>218</v>
       </c>
@@ -2941,7 +2947,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>228</v>
       </c>
@@ -2981,7 +2987,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>233</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>238</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>243</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>248</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>253</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>258</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>263</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>268</v>
       </c>
@@ -3141,7 +3147,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>273</v>
       </c>
@@ -3161,7 +3167,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>278</v>
       </c>
@@ -3181,7 +3187,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>283</v>
       </c>
@@ -3201,7 +3207,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="3" t="s">
         <v>288</v>
       </c>
@@ -3221,7 +3227,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="3" t="s">
         <v>293</v>
       </c>
@@ -3241,7 +3247,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="3" t="s">
         <v>298</v>
       </c>
@@ -3261,7 +3267,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="3" t="s">
         <v>303</v>
       </c>
@@ -3281,7 +3287,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="3" t="s">
         <v>308</v>
       </c>
@@ -3301,7 +3307,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="3" t="s">
         <v>313</v>
       </c>
@@ -3321,7 +3327,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="3" t="s">
         <v>318</v>
       </c>
@@ -3341,7 +3347,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="3" t="s">
         <v>323</v>
       </c>
@@ -3361,7 +3367,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="3" t="s">
         <v>328</v>
       </c>
@@ -3381,7 +3387,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="3" t="s">
         <v>333</v>
       </c>
@@ -3401,7 +3407,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="3" t="s">
         <v>338</v>
       </c>
@@ -3418,10 +3424,10 @@
         <v>342</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="3" t="s">
         <v>348</v>
       </c>
@@ -3438,10 +3444,10 @@
         <v>352</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="3" t="s">
         <v>353</v>
       </c>
@@ -3461,7 +3467,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="3" t="s">
         <v>361</v>
       </c>
@@ -3481,7 +3487,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="3" t="s">
         <v>371</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="3" t="s">
         <v>376</v>
       </c>
@@ -3521,7 +3527,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="3" t="s">
         <v>382</v>
       </c>
@@ -3541,7 +3547,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="3" t="s">
         <v>388</v>
       </c>
@@ -3561,7 +3567,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="3" t="s">
         <v>394</v>
       </c>
@@ -3581,7 +3587,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="3" t="s">
         <v>402</v>
       </c>
@@ -3601,7 +3607,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="3" t="s">
         <v>408</v>
       </c>
@@ -3621,7 +3627,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="3" t="s">
         <v>416</v>
       </c>
@@ -3641,7 +3647,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="3" t="s">
         <v>417</v>
       </c>
@@ -3661,7 +3667,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="3" t="s">
         <v>427</v>
       </c>
@@ -3681,7 +3687,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="3" t="s">
         <v>428</v>
       </c>
@@ -3701,7 +3707,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="3" t="s">
         <v>429</v>
       </c>
@@ -3721,7 +3727,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="3" t="s">
         <v>430</v>
       </c>
@@ -3741,7 +3747,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="3" t="s">
         <v>455</v>
       </c>
@@ -3761,7 +3767,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="3" t="s">
         <v>461</v>
       </c>
@@ -3781,7 +3787,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="3" t="s">
         <v>467</v>
       </c>

</xml_diff>

<commit_message>
update verbs.xlsx with changes
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259167B5-21FD-4813-9EDB-48085998384F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2D4130-E94A-4733-B904-08002A0E80B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="568">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -861,26 +861,10 @@
     <t>立ちます</t>
   </si>
   <si>
-    <t>戻す</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戻して</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戻した</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>戻さない</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>戻します</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>吸う</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1929,6 +1913,78 @@
   </si>
   <si>
     <t>届ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戻る</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戻って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戻った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戻ります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戻ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戻れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吹ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>降れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>なれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>遊べる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>着ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預けて</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預けた</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預けらない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預けます</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預けよう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預けられる</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2323,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2357,10 +2413,10 @@
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
@@ -2368,10 +2424,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -2380,10 +2436,10 @@
         <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2403,10 +2459,10 @@
         <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2426,10 +2482,10 @@
         <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2449,10 +2505,10 @@
         <v>34</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2472,10 +2528,10 @@
         <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2495,10 +2551,10 @@
         <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2518,10 +2574,10 @@
         <v>37</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2541,10 +2597,10 @@
         <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2564,10 +2620,10 @@
         <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2587,10 +2643,10 @@
         <v>52</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2610,10 +2666,10 @@
         <v>57</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2633,10 +2689,10 @@
         <v>62</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2656,10 +2712,10 @@
         <v>83</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2679,10 +2735,10 @@
         <v>85</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2702,10 +2758,10 @@
         <v>89</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2725,10 +2781,10 @@
         <v>77</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2748,10 +2804,10 @@
         <v>93</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2771,10 +2827,10 @@
         <v>97</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2794,10 +2850,10 @@
         <v>73</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2817,10 +2873,10 @@
         <v>102</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2840,10 +2896,10 @@
         <v>107</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2863,10 +2919,10 @@
         <v>112</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2886,10 +2942,10 @@
         <v>117</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2909,10 +2965,10 @@
         <v>122</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2932,10 +2988,10 @@
         <v>127</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2955,10 +3011,10 @@
         <v>132</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -2978,10 +3034,10 @@
         <v>137</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3001,10 +3057,10 @@
         <v>142</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3024,10 +3080,10 @@
         <v>147</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3047,10 +3103,10 @@
         <v>152</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3070,10 +3126,10 @@
         <v>157</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3093,10 +3149,10 @@
         <v>162</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3116,10 +3172,10 @@
         <v>167</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3139,1344 +3195,1367 @@
         <v>172</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>173</v>
-      </c>
-      <c r="B36" t="s">
-        <v>174</v>
+        <v>550</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>551</v>
       </c>
       <c r="C36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" t="s">
-        <v>176</v>
-      </c>
-      <c r="E36" t="s">
-        <v>177</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>359</v>
+        <v>552</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>554</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>546</v>
+        <v>555</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D37" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E37" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B38" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C38" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E38" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E39" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" t="s">
+        <v>190</v>
+      </c>
+      <c r="D40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
         <v>193</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>194</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>195</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>196</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>197</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>198</v>
-      </c>
-      <c r="B41" t="s">
-        <v>199</v>
-      </c>
-      <c r="C41" t="s">
-        <v>200</v>
-      </c>
-      <c r="D41" t="s">
-        <v>201</v>
-      </c>
-      <c r="E41" t="s">
-        <v>202</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>551</v>
+        <v>355</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>552</v>
+        <v>198</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>201</v>
       </c>
       <c r="E42" t="s">
-        <v>57</v>
+        <v>202</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>520</v>
+        <v>547</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>548</v>
       </c>
       <c r="B43" t="s">
-        <v>204</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>205</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>206</v>
+        <v>56</v>
       </c>
       <c r="E43" t="s">
-        <v>207</v>
+        <v>57</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>553</v>
+        <v>516</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" t="s">
+        <v>206</v>
+      </c>
+      <c r="E44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>208</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>209</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>210</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>211</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>212</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="F45" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>213</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>214</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>215</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>216</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>217</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>218</v>
-      </c>
-      <c r="B46" t="s">
-        <v>219</v>
-      </c>
-      <c r="C46" t="s">
-        <v>220</v>
-      </c>
-      <c r="D46" t="s">
-        <v>221</v>
-      </c>
-      <c r="E46" t="s">
-        <v>222</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>218</v>
+      </c>
+      <c r="B47" t="s">
+        <v>219</v>
+      </c>
+      <c r="C47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>223</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>224</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>225</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>226</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>227</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>228</v>
-      </c>
-      <c r="B48" t="s">
-        <v>229</v>
-      </c>
-      <c r="C48" t="s">
-        <v>230</v>
-      </c>
-      <c r="D48" t="s">
-        <v>231</v>
-      </c>
-      <c r="E48" t="s">
-        <v>232</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B49" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C49" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D49" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>359</v>
+        <v>560</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B50" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C50" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D50" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E50" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B51" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D51" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E51" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B52" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C52" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D52" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E52" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B53" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C53" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D53" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E53" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B54" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C54" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D54" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E54" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B55" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C55" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D55" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E55" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B56" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C56" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D56" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E56" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>268</v>
+      </c>
+      <c r="B57" t="s">
+        <v>269</v>
+      </c>
+      <c r="C57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" t="s">
+        <v>271</v>
+      </c>
+      <c r="E57" t="s">
+        <v>272</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>273</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>274</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>275</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>276</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>277</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="F58" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>287</v>
-      </c>
       <c r="F59" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>292</v>
-      </c>
       <c r="F60" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>297</v>
-      </c>
       <c r="F61" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>302</v>
-      </c>
       <c r="F62" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>307</v>
-      </c>
       <c r="F63" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="F64" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>317</v>
-      </c>
       <c r="F65" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="F66" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="F67" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>332</v>
-      </c>
       <c r="F68" s="4" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>341</v>
-      </c>
       <c r="F69" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>346</v>
-      </c>
       <c r="F70" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>354</v>
-      </c>
       <c r="F71" s="3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>364</v>
-      </c>
       <c r="F72" s="3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="F73" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>370</v>
-      </c>
       <c r="G73" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="F74" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>376</v>
-      </c>
       <c r="G74" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>382</v>
-      </c>
       <c r="G75" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>388</v>
-      </c>
       <c r="G76" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="F77" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>396</v>
-      </c>
       <c r="G77" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>402</v>
-      </c>
       <c r="G78" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>412</v>
-      </c>
       <c r="F79" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="D80" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>413</v>
-      </c>
       <c r="F80" s="3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="F81" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="G81" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="G82" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>435</v>
-      </c>
       <c r="G83" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>440</v>
-      </c>
       <c r="G84" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="F85" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>449</v>
-      </c>
       <c r="G85" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="F86" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>455</v>
-      </c>
       <c r="G86" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>460</v>
-      </c>
       <c r="F87" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E88" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="F88" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>468</v>
-      </c>
       <c r="G88" s="4" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="F89" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>480</v>
-      </c>
       <c r="G89" s="4" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>485</v>
-      </c>
       <c r="G90" s="4" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="F91" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>492</v>
-      </c>
       <c r="G91" s="4" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="F92" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>498</v>
-      </c>
       <c r="G92" s="3" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="D93" s="3" t="s">
+      <c r="F93" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="E93" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>504</v>
-      </c>
       <c r="G93" s="3" t="s">
-        <v>537</v>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A94" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor verb selection logic to ensure valid forms are chosen before adding to session
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F42E61-6112-4475-AE6A-FE78F8438748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FBD3A8-4A2B-412E-AE4F-8F51B246CD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="13980" yWindow="2370" windowWidth="12075" windowHeight="10935" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="604">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -2073,6 +2073,62 @@
   </si>
   <si>
     <t>はいれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出す</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出して</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出した</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出さない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出します</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出そう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引き出せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越す</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越して</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越した</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越さない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越します</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越そう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引っ越せる</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2467,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4692,6 +4748,52 @@
         <v>586</v>
       </c>
     </row>
+    <row r="97" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A97" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A98" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>603</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add ping endpoint and implement periodic check in frontend
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FBD3A8-4A2B-412E-AE4F-8F51B246CD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6058D6C-A3D8-41FC-84FB-E012FDC4B5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="2370" windowWidth="12075" windowHeight="10935" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="623">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -1880,10 +1880,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>触れる</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>戻せる</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2129,6 +2125,86 @@
   </si>
   <si>
     <t>引っ越せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>さわれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>走られる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>働ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>立てる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸える</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>降りられる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>咲ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>作れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>脱げる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>壊せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>閉まれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>止まれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>探せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾う</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾わない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾います</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾おう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾える</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2523,10 +2599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3342,30 +3418,30 @@
         <v>355</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>541</v>
+        <v>603</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
+        <v>549</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" t="s">
         <v>551</v>
-      </c>
-      <c r="C36" t="s">
-        <v>552</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>278</v>
       </c>
       <c r="E36" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>554</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3388,7 +3464,7 @@
         <v>355</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3411,7 +3487,7 @@
         <v>355</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3434,7 +3510,7 @@
         <v>355</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3457,7 +3533,7 @@
         <v>355</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3480,7 +3556,7 @@
         <v>355</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3503,12 +3579,12 @@
         <v>355</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
@@ -3549,7 +3625,7 @@
         <v>355</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3572,7 +3648,7 @@
         <v>355</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3595,7 +3671,7 @@
         <v>355</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3618,7 +3694,7 @@
         <v>355</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3641,7 +3717,7 @@
         <v>355</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3664,7 +3740,7 @@
         <v>355</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3687,7 +3763,7 @@
         <v>355</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3710,7 +3786,7 @@
         <v>355</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3733,7 +3809,7 @@
         <v>355</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3756,7 +3832,7 @@
         <v>355</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3779,7 +3855,7 @@
         <v>355</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3802,10 +3878,10 @@
         <v>355</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>263</v>
       </c>
@@ -3824,11 +3900,11 @@
       <c r="F56" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G56" s="4" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="3" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>268</v>
       </c>
@@ -3847,11 +3923,11 @@
       <c r="F57" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G57" s="4" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>273</v>
       </c>
@@ -3870,8 +3946,8 @@
       <c r="F58" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G58" s="4" t="s">
-        <v>355</v>
+      <c r="G58" s="3" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3893,8 +3969,8 @@
       <c r="F59" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>355</v>
+      <c r="G59" s="3" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3916,8 +3992,8 @@
       <c r="F60" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>355</v>
+      <c r="G60" s="3" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3939,8 +4015,8 @@
       <c r="F61" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>355</v>
+      <c r="G61" s="3" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3962,8 +4038,8 @@
       <c r="F62" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>355</v>
+      <c r="G62" s="3" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -3986,7 +4062,7 @@
         <v>355</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>355</v>
+        <v>611</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4008,8 +4084,8 @@
       <c r="F64" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G64" s="4" t="s">
-        <v>355</v>
+      <c r="G64" s="3" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4031,8 +4107,8 @@
       <c r="F65" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G65" s="4" t="s">
-        <v>355</v>
+      <c r="G65" s="3" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4054,8 +4130,8 @@
       <c r="F66" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G66" s="4" t="s">
-        <v>355</v>
+      <c r="G66" s="3" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4077,8 +4153,8 @@
       <c r="F67" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G67" s="4" t="s">
-        <v>355</v>
+      <c r="G67" s="3" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4492,7 +4568,7 @@
         <v>445</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4515,7 +4591,7 @@
         <v>451</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4681,117 +4757,140 @@
     </row>
     <row r="94" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="D94" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="F94" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>566</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="F95" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="F95" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="F96" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="G96" s="3" t="s">
         <v>585</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="F97" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="F97" s="3" t="s">
+      <c r="G97" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="F98" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="F98" s="3" t="s">
+      <c r="G98" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="G98" s="3" t="s">
-        <v>603</v>
+    </row>
+    <row r="99" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A99" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix load_words function to read from words.xlsx and add new words.xlsx file
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BA062E-5892-4B50-B619-8BFD5AE69996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DE6183-C3AD-4518-B068-14E44A48600A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="672">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -2316,6 +2316,89 @@
   </si>
   <si>
     <t>治れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落とす</t>
+  </si>
+  <si>
+    <t>落として</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落とした</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落とさない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落とします</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落とそう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落とせる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちて</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちた</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちます</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちよう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>落ちられる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残る</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残らない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残ります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残れる</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2710,10 +2793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5096,6 +5179,75 @@
         <v>650</v>
       </c>
     </row>
+    <row r="104" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>651</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A105" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A106" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>671</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update verbs.xlsx and words.xlsx with new data
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DE6183-C3AD-4518-B068-14E44A48600A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5F1235-836A-4573-A3CA-41EC7DEE8F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="696">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -2399,6 +2399,102 @@
   </si>
   <si>
     <t>残れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘う</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘わない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘います</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘おう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘える</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>渡れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>払える</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>謝れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>困れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>始まれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>終われる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>掛れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>押せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>渡せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>とおれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かよえる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下ろせる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がれる</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2793,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2808,6 +2904,7 @@
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4370,8 +4467,8 @@
       <c r="F68" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="G68" s="4" t="s">
-        <v>355</v>
+      <c r="G68" s="3" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4393,8 +4490,8 @@
       <c r="F69" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="G69" s="4" t="s">
-        <v>355</v>
+      <c r="G69" s="3" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4416,8 +4513,8 @@
       <c r="F70" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G70" s="4" t="s">
-        <v>355</v>
+      <c r="G70" s="3" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4439,8 +4536,8 @@
       <c r="F71" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="G71" s="4" t="s">
-        <v>355</v>
+      <c r="G71" s="3" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4462,8 +4559,8 @@
       <c r="F72" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="G72" s="4" t="s">
-        <v>355</v>
+      <c r="G72" s="3" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4485,8 +4582,8 @@
       <c r="F73" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>355</v>
+      <c r="G73" s="3" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4509,7 +4606,7 @@
         <v>372</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>355</v>
+        <v>685</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4531,8 +4628,8 @@
       <c r="F75" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="G75" s="4" t="s">
-        <v>355</v>
+      <c r="G75" s="3" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4554,8 +4651,8 @@
       <c r="F76" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="G76" s="4" t="s">
-        <v>355</v>
+      <c r="G76" s="3" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4578,7 +4675,7 @@
         <v>392</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>355</v>
+        <v>688</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4600,8 +4697,8 @@
       <c r="F78" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G78" s="4" t="s">
-        <v>355</v>
+      <c r="G78" s="3" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4623,8 +4720,8 @@
       <c r="F79" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="G79" s="4" t="s">
-        <v>355</v>
+      <c r="G79" s="3" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4646,8 +4743,8 @@
       <c r="F80" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="G80" s="4" t="s">
-        <v>355</v>
+      <c r="G80" s="3" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4669,8 +4766,8 @@
       <c r="F81" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="G81" s="4" t="s">
-        <v>355</v>
+      <c r="G81" s="3" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4692,8 +4789,8 @@
       <c r="F82" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="G82" s="4" t="s">
-        <v>355</v>
+      <c r="G82" s="3" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4715,8 +4812,8 @@
       <c r="F83" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="G83" s="4" t="s">
-        <v>355</v>
+      <c r="G83" s="3" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4738,8 +4835,8 @@
       <c r="F84" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="G84" s="4" t="s">
-        <v>355</v>
+      <c r="G84" s="3" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -5246,6 +5343,29 @@
       </c>
       <c r="G106" s="3" t="s">
         <v>671</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update verbs.xlsx and words.xlsx with recent changes
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DE6183-C3AD-4518-B068-14E44A48600A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFADB37-C7C7-45C1-BF42-F8A15DCC73AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="714">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -2399,6 +2399,174 @@
   </si>
   <si>
     <t>残れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘う</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘わない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘います</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘おう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>誘える</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>渡れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>払える</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>謝れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>困れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>始まれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>終われる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>掛れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>押せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>渡せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返せる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>焼ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>とおれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>かよえる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>送れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上がれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下ろせる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下がれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答える</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答えて</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答えた</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答えない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答えます</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答えよう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答えられる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passive Form</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行こう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行ける</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行かれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残す</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残して</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残した</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残さない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残します</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残そう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>残せる</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2793,10 +2961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2808,9 +2976,10 @@
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2832,8 +3001,11 @@
       <c r="G1" s="1" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2850,13 +3022,16 @@
         <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>330</v>
+        <v>704</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+        <v>705</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2879,7 +3054,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2902,7 +3077,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2925,7 +3100,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2948,7 +3123,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2971,7 +3146,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -2994,7 +3169,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -3017,7 +3192,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -3040,7 +3215,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -3063,7 +3238,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
@@ -3086,7 +3261,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -3109,7 +3284,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -3132,7 +3307,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -3155,7 +3330,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4370,8 +4545,8 @@
       <c r="F68" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="G68" s="4" t="s">
-        <v>355</v>
+      <c r="G68" s="3" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4393,8 +4568,8 @@
       <c r="F69" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="G69" s="4" t="s">
-        <v>355</v>
+      <c r="G69" s="3" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4416,8 +4591,8 @@
       <c r="F70" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="G70" s="4" t="s">
-        <v>355</v>
+      <c r="G70" s="3" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4439,8 +4614,8 @@
       <c r="F71" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="G71" s="4" t="s">
-        <v>355</v>
+      <c r="G71" s="3" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4462,8 +4637,8 @@
       <c r="F72" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="G72" s="4" t="s">
-        <v>355</v>
+      <c r="G72" s="3" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4485,8 +4660,8 @@
       <c r="F73" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>355</v>
+      <c r="G73" s="3" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4509,7 +4684,7 @@
         <v>372</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>355</v>
+        <v>685</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4531,8 +4706,8 @@
       <c r="F75" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="G75" s="4" t="s">
-        <v>355</v>
+      <c r="G75" s="3" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4554,8 +4729,8 @@
       <c r="F76" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="G76" s="4" t="s">
-        <v>355</v>
+      <c r="G76" s="3" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4578,7 +4753,7 @@
         <v>392</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>355</v>
+        <v>688</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4600,8 +4775,8 @@
       <c r="F78" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G78" s="4" t="s">
-        <v>355</v>
+      <c r="G78" s="3" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4623,8 +4798,8 @@
       <c r="F79" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="G79" s="4" t="s">
-        <v>355</v>
+      <c r="G79" s="3" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4646,8 +4821,8 @@
       <c r="F80" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="G80" s="4" t="s">
-        <v>355</v>
+      <c r="G80" s="3" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4669,8 +4844,8 @@
       <c r="F81" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="G81" s="4" t="s">
-        <v>355</v>
+      <c r="G81" s="3" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4692,8 +4867,8 @@
       <c r="F82" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="G82" s="4" t="s">
-        <v>355</v>
+      <c r="G82" s="3" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4715,8 +4890,8 @@
       <c r="F83" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="G83" s="4" t="s">
-        <v>355</v>
+      <c r="G83" s="3" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -4738,8 +4913,8 @@
       <c r="F84" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="G84" s="4" t="s">
-        <v>355</v>
+      <c r="G84" s="3" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -5246,6 +5421,75 @@
       </c>
       <c r="G106" s="3" t="s">
         <v>671</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A108" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A109" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update verbs.xlsx with recent changes
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mptang\Desktop\local testing\online-web-app-deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADC2F69-A063-4D3C-9EE5-5AB95DA6F6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BDF84A-FDD9-41CD-9A3E-B5B30AA5F3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31845" yWindow="3705" windowWidth="21600" windowHeight="11295" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="745">
   <si>
     <t>Dictionary Form</t>
   </si>
@@ -2610,17 +2610,85 @@
   </si>
   <si>
     <t>巻き込める</t>
+  </si>
+  <si>
+    <t>怒る</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒って</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒った</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒らない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒ります</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒ろう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒れる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>怒られる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>巻き込まれる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行われる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きて</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きた</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きない</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きます</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きよう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生きられる</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2629,14 +2697,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2691,7 +2759,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2707,9 +2775,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2747,7 +2815,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2853,7 +2921,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2995,7 +3063,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3003,13 +3071,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -3021,7 +3089,7 @@
     <col min="8" max="8" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3047,7 +3115,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3073,7 +3141,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3096,7 +3164,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -3119,7 +3187,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3142,7 +3210,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -3165,7 +3233,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -3188,7 +3256,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -3211,7 +3279,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75">
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -3234,7 +3302,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75">
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -3257,7 +3325,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75">
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -3280,7 +3348,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75">
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
@@ -3303,7 +3371,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -3326,7 +3394,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75">
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -3349,7 +3417,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75">
+    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -3372,7 +3440,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75">
+    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -3395,7 +3463,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -3418,7 +3486,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75">
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -3441,7 +3509,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75">
+    <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -3464,7 +3532,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -3487,7 +3555,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -3510,7 +3578,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75">
+    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -3533,7 +3601,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75">
+    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -3556,7 +3624,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75">
+    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -3579,7 +3647,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75">
+    <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -3602,7 +3670,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75">
+    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -3625,7 +3693,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75">
+    <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -3648,7 +3716,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75">
+    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3671,7 +3739,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -3694,7 +3762,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3717,7 +3785,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18.75">
+    <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -3740,7 +3808,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -3763,7 +3831,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18.75">
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -3786,7 +3854,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18.75">
+    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -3809,7 +3877,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="18.75">
+    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -3832,7 +3900,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="18.75">
+    <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>549</v>
       </c>
@@ -3855,7 +3923,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="18.75">
+    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -3878,7 +3946,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="18.75">
+    <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -3901,7 +3969,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="18.75">
+    <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>183</v>
       </c>
@@ -3924,7 +3992,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="18.75">
+    <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>188</v>
       </c>
@@ -3947,7 +4015,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="18.75">
+    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>193</v>
       </c>
@@ -3970,7 +4038,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>198</v>
       </c>
@@ -3993,7 +4061,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>547</v>
       </c>
@@ -4016,7 +4084,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>203</v>
       </c>
@@ -4039,7 +4107,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="18.75">
+    <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4062,7 +4130,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18.75">
+    <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>213</v>
       </c>
@@ -4085,7 +4153,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>218</v>
       </c>
@@ -4108,7 +4176,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="18.75">
+    <row r="48" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>223</v>
       </c>
@@ -4131,7 +4199,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>228</v>
       </c>
@@ -4154,7 +4222,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>233</v>
       </c>
@@ -4177,7 +4245,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>238</v>
       </c>
@@ -4200,7 +4268,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>243</v>
       </c>
@@ -4223,7 +4291,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18.75">
+    <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>248</v>
       </c>
@@ -4246,7 +4314,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -4269,7 +4337,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18.75">
+    <row r="55" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>258</v>
       </c>
@@ -4292,7 +4360,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18.75">
+    <row r="56" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>263</v>
       </c>
@@ -4315,7 +4383,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18.75">
+    <row r="57" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>268</v>
       </c>
@@ -4338,7 +4406,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="18.75">
+    <row r="58" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>273</v>
       </c>
@@ -4361,7 +4429,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="18.75">
+    <row r="59" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>279</v>
       </c>
@@ -4384,7 +4452,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18.75">
+    <row r="60" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>284</v>
       </c>
@@ -4407,7 +4475,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="18.75">
+    <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>289</v>
       </c>
@@ -4430,7 +4498,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="18.75">
+    <row r="62" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>294</v>
       </c>
@@ -4453,7 +4521,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18.75">
+    <row r="63" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>299</v>
       </c>
@@ -4476,7 +4544,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="18.75">
+    <row r="64" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>304</v>
       </c>
@@ -4499,7 +4567,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18.75">
+    <row r="65" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>309</v>
       </c>
@@ -4522,7 +4590,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="18.75">
+    <row r="66" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
         <v>314</v>
       </c>
@@ -4545,7 +4613,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="18.75">
+    <row r="67" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>319</v>
       </c>
@@ -4568,7 +4636,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="18.75">
+    <row r="68" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
         <v>324</v>
       </c>
@@ -4591,7 +4659,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="18.75">
+    <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
         <v>333</v>
       </c>
@@ -4614,7 +4682,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="18.75">
+    <row r="70" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>338</v>
       </c>
@@ -4637,7 +4705,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="18.75">
+    <row r="71" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
         <v>346</v>
       </c>
@@ -4660,7 +4728,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="18.75">
+    <row r="72" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>356</v>
       </c>
@@ -4683,7 +4751,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="18.75">
+    <row r="73" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>361</v>
       </c>
@@ -4706,7 +4774,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="18.75">
+    <row r="74" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>367</v>
       </c>
@@ -4729,7 +4797,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="18.75">
+    <row r="75" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>373</v>
       </c>
@@ -4752,7 +4820,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="18.75">
+    <row r="76" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>379</v>
       </c>
@@ -4775,7 +4843,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="18.75">
+    <row r="77" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>387</v>
       </c>
@@ -4798,7 +4866,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="18.75">
+    <row r="78" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>393</v>
       </c>
@@ -4821,7 +4889,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="18.75">
+    <row r="79" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>401</v>
       </c>
@@ -4844,7 +4912,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="18.75">
+    <row r="80" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>402</v>
       </c>
@@ -4867,7 +4935,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18.75">
+    <row r="81" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>412</v>
       </c>
@@ -4890,7 +4958,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="18.75">
+    <row r="82" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>413</v>
       </c>
@@ -4913,7 +4981,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="18.75">
+    <row r="83" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>414</v>
       </c>
@@ -4936,7 +5004,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="18.75">
+    <row r="84" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>415</v>
       </c>
@@ -4959,7 +5027,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="18.75">
+    <row r="85" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>440</v>
       </c>
@@ -4982,7 +5050,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="18.75">
+    <row r="86" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>446</v>
       </c>
@@ -5005,7 +5073,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18.75">
+    <row r="87" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>452</v>
       </c>
@@ -5028,7 +5096,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="18.75">
+    <row r="88" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
         <v>459</v>
       </c>
@@ -5051,7 +5119,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="18.75">
+    <row r="89" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
         <v>471</v>
       </c>
@@ -5074,7 +5142,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="18.75">
+    <row r="90" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
         <v>477</v>
       </c>
@@ -5097,7 +5165,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="18.75">
+    <row r="91" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>483</v>
       </c>
@@ -5120,7 +5188,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18.75">
+    <row r="92" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>489</v>
       </c>
@@ -5143,7 +5211,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="18.75">
+    <row r="93" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>495</v>
       </c>
@@ -5166,7 +5234,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="18.75">
+    <row r="94" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>560</v>
       </c>
@@ -5189,7 +5257,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="18.75">
+    <row r="95" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>572</v>
       </c>
@@ -5212,7 +5280,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="18.75">
+    <row r="96" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>579</v>
       </c>
@@ -5235,7 +5303,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="18.75">
+    <row r="97" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>589</v>
       </c>
@@ -5258,7 +5326,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="18.75">
+    <row r="98" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
         <v>596</v>
       </c>
@@ -5281,7 +5349,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="18.75">
+    <row r="99" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
         <v>616</v>
       </c>
@@ -5304,7 +5372,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="18.75">
+    <row r="100" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
         <v>623</v>
       </c>
@@ -5327,7 +5395,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18.75">
+    <row r="101" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>630</v>
       </c>
@@ -5350,7 +5418,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="18.75">
+    <row r="102" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
         <v>637</v>
       </c>
@@ -5373,7 +5441,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="18.75">
+    <row r="103" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
         <v>644</v>
       </c>
@@ -5396,7 +5464,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="18.75">
+    <row r="104" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>651</v>
       </c>
@@ -5419,7 +5487,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="18.75">
+    <row r="105" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
         <v>658</v>
       </c>
@@ -5442,7 +5510,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="18.75">
+    <row r="106" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
         <v>665</v>
       </c>
@@ -5465,7 +5533,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="18.75">
+    <row r="107" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
         <v>672</v>
       </c>
@@ -5488,7 +5556,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="18.75">
+    <row r="108" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
         <v>696</v>
       </c>
@@ -5511,7 +5579,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="18.75">
+    <row r="109" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
         <v>707</v>
       </c>
@@ -5534,7 +5602,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="18.75">
+    <row r="110" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
         <v>714</v>
       </c>
@@ -5556,8 +5624,11 @@
       <c r="G110" s="3" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="18.75">
+      <c r="H110" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
         <v>721</v>
       </c>
@@ -5578,6 +5649,61 @@
       </c>
       <c r="G111" s="3" t="s">
         <v>727</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A112" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A113" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>